<commit_message>
removed empty field feature
</commit_message>
<xml_diff>
--- a/uploads/scrapped.xlsx
+++ b/uploads/scrapped.xlsx
@@ -390,10 +390,10 @@
     </row>
     <row r="2" xml:space="preserve">
       <c r="A2" t="str">
-        <v>S</v>
+        <v>A</v>
       </c>
       <c r="B2" t="str" xml:space="preserve">
-        <v xml:space="preserve">S, or s, is the nineteenth letter in the Modern English alphabet and the ISO basic Latin alphabet. Its name in English is ess[1] (pronounced /ˈɛs/), plural esses.[2]
+        <v xml:space="preserve">A, or a, is the first letter and the first vowel of the modern English alphabet and the ISO basic Latin alphabet.[1][2] Its name in English is a (pronounced /ˈeɪ/), plural aes.[nb 1] It is similar in shape to the Ancient Greek letter alpha, from which it derives.[3] The uppercase version consists of the two slanting sides of a triangle, crossed in the middle by a horizontal bar. The lowercase version can be written in two forms: the double-storey a and single-storey ɑ. The latter is commonly used in handwriting and fonts based on it, especially fonts intended to be read by children, and is also found in italic type.
 </v>
       </c>
     </row>
@@ -402,24 +402,13 @@
         <v>History</v>
       </c>
       <c r="B3" t="str" xml:space="preserve">
-        <v xml:space="preserve">OriginNorthwest Semitic šîn  represented a voiceless postalveolar fricative /ʃ/ (as in 'ship'). It originated most likely as a pictogram of a tooth (שנא) and represented the phoneme /ʃ/ via the acrophonic principle.[3]
-Ancient Greek did not have a  /ʃ/ phoneme, so the derived Greek letter sigma (Σ) came to represent the voiceless alveolar sibilant /s/. 
-While the letter shape Σ continues Phoenician šîn, its name sigma is taken from the letter samekh, while the shape and position of samekh but name of šîn is continued in the xi.[citation needed]
-Within Greek, the name of sigma was influenced by its association with the Greek word σίζω (earlier *sigj-) "to hiss". The original name of the letter "sigma" may have been san, but due to the complicated early history of the Greek epichoric alphabets, "san" came to be identified as a separate letter, Ϻ.[4] Herodotus reports that "San" was the name given by the  Dorians to the same letter called "Sigma" by the Ionians.[5]
-The Western Greek alphabet used in Cumae was adopted by the Etruscans and Latins in the 7th century BC, over the following centuries developing into a range of Old Italic alphabets including the Etruscan alphabet and the early Latin alphabet.
-In Etruscan, the value /s/ of Greek sigma (𐌔) was maintained, while san (𐌑)
-represented a separate phoneme, most likely /ʃ/ (transliterated as ś). 
-The early Latin alphabet adopted sigma, but not san, as Old Latin did not have a  /ʃ/ phoneme.
-The shape of Latin S arises from Greek Σ by dropping one out of the four strokes of that letter.
-The (angular) S-shape composed of three strokes existed as a variant of the four-stroke letter Σ already in the epigraphy in Western Greek alphabets, and the three and four strokes variants existed alongside one another in the classical Etruscan alphabet. In other Italic alphabets (Venetic, Lepontic), the letter could be represented as a zig-zagging line of any number between three and six strokes.
-The Italic letter was also adopted into Elder Futhark, as Sowilō (ᛊ), and appears with four to eight strokes in the earliest runic inscriptions, but is occasionally reduced to three strokes (ᛋ) from the later 5th century, and appears regularly with three strokes in Younger Futhark.
-Long sThe minuscule form  ſ, called the long s, developed in the early medieval period, within the Visigothic and Carolingian hands, with predecessors in the half-uncial and cursive scripts of Late Antiquity. It remained standard in western writing throughout the medieval period and was adopted in early printing with movable types. 
-It existed alongside minuscule "round" or "short" s, which was at the time only used at the end of words.
-In most western orthographies, the ſ gradually fell out of use during the second half of the 18th century, although it remained in occasional use into the 19th century.
-In Spain, the change was mainly accomplished between the years 1760 and 1766. In France, the change occurred between 1782 and 1793. Printers in the United States stopped using the long s between 1795 and 1810. In English orthography, the London printer John Bell (1745–1831) pioneered the change. His edition of Shakespeare, in 1785, was advertised with the claim that he "ventured to depart from the common mode by rejecting the long 'ſ' in favor of the round one, as being less liable to error....."[6]   The Times of London made the switch from the long to the short s with its issue of 10 September 1803. 
-Encyclopædia Britannica's 5th edition, completed in 1817, was the last edition to use the long s.
-In German orthography, long s was retained in Fraktur (Schwabacher) type as well as in standard cursive (Sütterlin) well into the 20th century, and was officially abolished in 1941.[7]
-The ligature of ſs (or ſz) was retained, however, giving rise to the Eszett, ß in contemporary German orthography.
+        <v xml:space="preserve">The earliest certain ancestor of "A" is aleph (also written 'aleph), the first letter of the Phoenician alphabet,[4] which consisted entirely of consonants (for that reason, it is also called an abjad to distinguish it from a true alphabet). In turn, the ancestor of aleph may have been a pictogram of an ox head in proto-Sinaitic script[5] influenced by Egyptian hieroglyphs, styled as a triangular head with two horns extended.
+When the ancient Greeks adopted the alphabet, they had no use for a letter to represent the glottal stop—the consonant sound that the letter denoted in Phoenician and other Semitic languages, and that was the first phoneme of the Phoenician pronunciation of the letter—so they used their version of the sign to represent the vowel /a/, and called it by the similar name of alpha. In the earliest Greek inscriptions after the Greek Dark Ages, dating to the 8th century BC, the letter rests upon its side, but in the Greek alphabet of later times it generally resembles the modern capital letter, although many local varieties can be distinguished by the shortening of one leg, or by the angle at which the cross line is set.
+The Etruscans brought the Greek alphabet to their civilization in the Italian Peninsula and left the letter unchanged. The Romans later adopted the Etruscan alphabet to write the Latin language, and the resulting letter was preserved in the Latin alphabet that would come to be used to write many languages, including English.
+Typographic variantsDuring Roman times, there were many variant forms of the letter "A". First was the monumental or lapidary style, which was used when inscribing on stone or other "permanent" media. There was also a cursive style used for everyday or utilitarian writing, which was done on more perishable surfaces. Due to the "perishable" nature of these surfaces, there are not as many examples of this style as there are of the monumental, but there are still many surviving examples of different types of cursive, such as majuscule cursive, minuscule cursive, and semicursive minuscule. Variants also existed that were intermediate between the monumental and cursive styles. The known variants include the early semi-uncial, the uncial, and the later semi-uncial.[6]
+At the end of the Roman Empire (5th century AD), several variants of the cursive minuscule developed through Western Europe. Among these were the semicursive minuscule of Italy, the Merovingian script in France, the Visigothic script in Spain, and the Insular or Anglo-Irish semi-uncial or Anglo-Saxon majuscule of Great Britain. By the 9th century, the Caroline script, which was very similar to the present-day form, was the principal form used in book-making, before the advent of the printing press. This form was derived through a combining of prior forms.[6]
+15th-century Italy saw the formation of the two main variants that are known today. These variants, the Italic and Roman forms, were derived from the Caroline Script version. The Italic form, also called script a, is used in most current handwriting; it consists of a circle and vertical stroke on the right ("ɑ"). This slowly developed from the fifth-century form resembling the Greek letter tau in the hands of medieval Irish and English writers.[4] The Roman form is used in most printed material; it consists of a small loop with an arc over it ("a").[6] Both derive from the majuscule (capital) form. In Greek handwriting, it was common to join the left leg and horizontal stroke into a single loop, as demonstrated by the uncial version shown. Many fonts then made the right leg vertical. In some of these, the serif that began the right leg stroke developed into an arc, resulting in the printed form, while in others it was dropped, resulting in the modern handwritten form. Graphic designers refer to the Italic and Roman forms as "single decker a" and "double decker a" respectively.
+Italic type is commonly used to mark emphasis or more generally to distinguish one part of a text from the rest (set in Roman type). There are some other cases aside from italic type where script a ("ɑ"), also called Latin alpha, is used in contrast with Latin "a" (such as in the International Phonetic Alphabet).
 </v>
       </c>
     </row>
@@ -428,43 +417,33 @@
         <v>Use in writing systems</v>
       </c>
       <c r="B4" t="str" xml:space="preserve">
-        <v xml:space="preserve">The letter ⟨s⟩ is the seventh most common letter in English and the third-most common consonant after ⟨t⟩ and ⟨n⟩.[8] It is the most common letter for the first letter of a word in the English language.[9][10]
-In English and several other languages, primarily Western Romance ones like Spanish and French, final ⟨s⟩ is the usual mark of plural nouns. It is the regular ending of English third person present tense verbs.
-⟨s⟩ represents the voiceless alveolar or voiceless dental sibilant /s/ in most languages as well as in the International Phonetic Alphabet. It also commonly represents the voiced alveolar or voiced dental sibilant /z/, as in Portuguese mesa (table) or English 'rose' and 'bands', or it may represent the voiceless palato-alveolar fricative [ʃ], as in most Portuguese dialects when syllable-finally, in Hungarian, in German (before ⟨p⟩, ⟨t⟩) and some English words as 'sugar', since yod-coalescence became a dominant feature, and [ʒ], as in English 'measure' (also because of yod-coalescence), European Portuguese Islão (Islam) or, in many sociolects of Brazilian Portuguese, esdrúxulo (proparoxytone) in some Andalusian dialects, it merged with Peninsular Spanish ⟨c⟩ and ⟨z⟩ and is now pronounced [θ].  In some English words of French origin, the letter ⟨s⟩ is silent, as in 'isle' or 'debris'. In Turkmen, ⟨s⟩ represents [θ].
-The ⟨sh⟩ digraph for English  /ʃ/ arises in Middle English (alongside ⟨sch⟩), replacing the Old English ⟨sc⟩ digraph. Similarly, Old High German ⟨sc⟩ was replaced by ⟨sch⟩ in Early Modern High German orthography.
-</v>
+        <v xml:space="preserve">EnglishIn modern English orthography, the letter ⟨a⟩ represents at least seven different vowel sounds:
+the near-open front unrounded vowel /æ/ as in pad;
+the open back unrounded vowel /ɑː/ as in father, which is closer to its original Latin and Greek sound;[5]
+the diphthong /eɪ/ as in ace and major (usually when ⟨a⟩ is followed by one, or occasionally two, consonants and then another vowel letter) – this results from Middle English lengthening followed by the Great Vowel Shift;
+the modified form of the above sound that occurs before ⟨r⟩, as in square and Mary;
+the rounded vowel of water;
+the shorter rounded vowel (not present in General American) in was and what;[4]
+a schwa, in many unstressed syllables, as in about, comma, solar.The double ⟨aa⟩ sequence does not occur in native English words, but is found in some words derived from foreign languages such as Aaron and aardvark.[7] However, ⟨a⟩ occurs in many common digraphs, all with their own sound or sounds, particularly ⟨ai⟩, ⟨au⟩, ⟨aw⟩, ⟨ay⟩, ⟨ea⟩ and ⟨oa⟩.
+⟨a⟩ is the third-most-commonly used letter in English (after ⟨e⟩ and ⟨t⟩),[8] and the second most common in Spanish and French. In one study, on average, about 3.68% of letters used in English texts tend to be ⟨a⟩, while the number is 6.22% in Spanish and 3.95% in French.[8]
+Other languagesIn most languages that use the Latin alphabet, ⟨a⟩ denotes an open unrounded vowel, such as /a/, /ä/, or /ɑ/. An exception is Saanich, in which ⟨a⟩ (and the glyph Á) stands for a close-mid front unrounded vowel /e/.
+Other systemsIn phonetic and phonemic notation:
+in the International Phonetic Alphabet, ⟨a⟩ is used for the open front unrounded vowel, ⟨ä⟩ is used for the open central unrounded vowel, and ⟨ɑ⟩ is used for the open back unrounded vowel.
+in X-SAMPA, ⟨a⟩ is used for the open front unrounded vowel and ⟨A⟩ is used for the open back unrounded vowel.</v>
       </c>
     </row>
     <row r="5" xml:space="preserve">
       <c r="A5" t="str">
-        <v>Related characters</v>
+        <v>Other uses</v>
       </c>
       <c r="B5" t="str" xml:space="preserve">
-        <v xml:space="preserve">Descendants and related characters in the Latin alphabetſ : Latin letter long s, an obsolete variant of s
-ẜ ẝ : Various forms of long s were used for medieval scribal abbreviations[11]
-ẞ ß : German Eszett or "sharp S", derived from a ligature of long s followed by either s or z
-S with diacritics: Ś ś Ṡ ṡ ẛ Ṩ ṩ Ṥ ṥ Ṣ ṣ S̩ s̩ Ꞩ ꞩ Ꟊꟊ[12] Ŝ ŝ Ṧ ṧ Š š Ş ş Ș ș S̈ s̈ ᶊ Ȿ ȿ ᵴ[13] ᶳ[14]
-ₛ : Subscript small s was used in the Uralic Phonetic Alphabet prior to its formal standardization in 1902[15]
-ˢ : Modifier letter small s is used for phonetic transcription
-ꜱ : Small capital S was used in the Icelandic First Grammatical Treatise to mark gemination[11]
-Ʂ ʂ : S with hook, used for writing Mandarin Chinese using the early draft version of pinyin romanization during the mid-1950s[16]
-Ƨ ƨ : Latin letter reversed S (used in Zhuang transliteration)
-IPA-specific symbols related to S: ʃ ɧ[citation needed] ʂ
-Ꞅ ꞅ : Insular SDerived signs, symbols, and abbreviations$ : Dollar sign
-₷ : Spesmilo
-§ : Section sign
-℠ : Service mark symbol
-∫ : Integral symbol, short for summation (derived from long s)Ancestors and siblings in other alphabets𐤔 : Semitic letter Shin, from which the following symbols originally derive
-archaic Greek Sigma could be written with different numbers of angles and strokes. Besides the classical form with four strokes (), a three-stroke form resembling an angular Latin S () was commonly found, and was particularly characteristic of some mainland Greek varieties including Attic and several "red" alphabets.
-Σ: classical Greek letter Sigma
-Ϲ ϲ: Greek lunate sigma
-Ⲥ ⲥ : Coptic letter sima
-С с : Cyrillic letter Es, derived from a form of sigma
-𐌔 : Old Italic letter S, includes the variants also found in the archaic Greek letter
-S: Latin letter S
-ᛊ, ᛋ, ᛌ : Runic letter sowilo, which is derived from Old Italic S
-𐍃: Gothic letter sigil
-Ս : Armenian letter Se</v>
+        <v xml:space="preserve">In algebra, the letter a along with various other letters of the alphabet is often used to denote a variable, with various conventional meanings in different areas of mathematics. Moreover, in 1637, René Descartes "invented the convention of representing unknowns in equations by x, y, and z, and knowns by a, b, and c",[9] and this convention is still often followed, especially in elementary algebra.
+In geometry, capital A, B, C etc. are used to denote segments, lines, rays, etc.[6] A capital A is also typically used as one of the letters to represent an angle in a triangle, the lowercase a representing the side opposite angle A.[5]
+"A" is often used to denote something or someone of a better or more prestigious quality or status: A-, A or A+, the best grade that can be assigned by teachers for students' schoolwork; "A grade" for clean restaurants; A-list celebrities, etc. Such associations can have a motivating effect, as exposure to the letter A has been found to improve performance, when compared with other letters.[10]
+"A" is used as a prefix on some words, such as asymmetry, to mean "not" or "without" (from Greek).
+In English grammar, "a", and its variant "an", is an indefinite article, used to introduce noun phrases.
+Finally, the letter A is used to denote size, as in a narrow size shoe,[5] or a small cup size in a brassiere.[11]
+</v>
       </c>
     </row>
   </sheetData>

</xml_diff>